<commit_message>
Made blocks list comprehesions
</commit_message>
<xml_diff>
--- a/geo_input.csv.xlsx
+++ b/geo_input.csv.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="123">
   <si>
     <t/>
   </si>
@@ -32,58 +32,109 @@
     <t>TUR</t>
   </si>
   <si>
-    <t>No response from data source</t>
+    <t>iShares MSCI Turk</t>
   </si>
   <si>
     <t>EPHE</t>
   </si>
   <si>
+    <t>iShares MSCI Phil</t>
+  </si>
+  <si>
     <t>EGPT</t>
   </si>
   <si>
+    <t>Market Vectors Eg</t>
+  </si>
+  <si>
+    <t>GERJ</t>
+  </si>
+  <si>
+    <t>Market Vectors Ge</t>
+  </si>
+  <si>
+    <t>THD</t>
+  </si>
+  <si>
+    <t>iShares MSCI Thai</t>
+  </si>
+  <si>
     <t>EPOL</t>
   </si>
   <si>
-    <t>THD</t>
+    <t>iShares MSCI Pola</t>
+  </si>
+  <si>
+    <t>EWW</t>
+  </si>
+  <si>
+    <t>iShares MSCI Mexi</t>
+  </si>
+  <si>
+    <t>EIRL</t>
+  </si>
+  <si>
+    <t>MSCI Ireland Capp</t>
+  </si>
+  <si>
+    <t>VNM</t>
+  </si>
+  <si>
+    <t>Market Vectors Vi</t>
   </si>
   <si>
     <t>PLND</t>
   </si>
   <si>
-    <t>GERJ</t>
-  </si>
-  <si>
-    <t>EIRL</t>
-  </si>
-  <si>
-    <t>EWW</t>
+    <t>Market Vectors Po</t>
+  </si>
+  <si>
+    <t>SCIF</t>
+  </si>
+  <si>
+    <t>MV India Small-Ca</t>
   </si>
   <si>
     <t>EWG</t>
   </si>
   <si>
+    <t>iShares MSCI Germ</t>
+  </si>
+  <si>
     <t>EWS</t>
   </si>
   <si>
+    <t>iShares MSCI Sing</t>
+  </si>
+  <si>
     <t>ENZL</t>
   </si>
   <si>
+    <t>iShares MSCI New</t>
+  </si>
+  <si>
     <t>EWO</t>
   </si>
   <si>
+    <t>iShares MSCI Aust</t>
+  </si>
+  <si>
     <t>EWH</t>
   </si>
   <si>
-    <t>SCIF</t>
+    <t>iShares MSCI Hong</t>
   </si>
   <si>
     <t>INDY</t>
   </si>
   <si>
+    <t>iShares S&amp;P India</t>
+  </si>
+  <si>
     <t>EPP</t>
   </si>
   <si>
-    <t>VNM</t>
+    <t>iShares MSCI Paci</t>
   </si>
   <si>
     <t>AFK</t>
@@ -92,144 +143,234 @@
     <t>Market Vectors-Af</t>
   </si>
   <si>
+    <t>FCHI</t>
+  </si>
+  <si>
+    <t>iShares FTSE Chin</t>
+  </si>
+  <si>
+    <t>MCHI</t>
+  </si>
+  <si>
+    <t>iShares MSCI Chin</t>
+  </si>
+  <si>
+    <t>EPU</t>
+  </si>
+  <si>
+    <t>iShares MSCI All</t>
+  </si>
+  <si>
+    <t>COLX</t>
+  </si>
+  <si>
+    <t>Market Vectors Co</t>
+  </si>
+  <si>
     <t>EWD</t>
   </si>
   <si>
+    <t>iShares MSCI Swed</t>
+  </si>
+  <si>
+    <t>EWA</t>
+  </si>
+  <si>
+    <t>AAXJ</t>
+  </si>
+  <si>
     <t>EWQ</t>
   </si>
   <si>
-    <t>EWA</t>
-  </si>
-  <si>
-    <t>AAXJ</t>
-  </si>
-  <si>
-    <t>iShares MSCI All</t>
-  </si>
-  <si>
-    <t>EPU</t>
-  </si>
-  <si>
-    <t>COLX</t>
-  </si>
-  <si>
-    <t>Market Vectors Co</t>
-  </si>
-  <si>
-    <t>MCHI</t>
-  </si>
-  <si>
-    <t>FCHI</t>
+    <t>iShares MSCI Fran</t>
+  </si>
+  <si>
+    <t>EWL</t>
+  </si>
+  <si>
+    <t>iShares MSCI Swit</t>
   </si>
   <si>
     <t>EDEN</t>
   </si>
   <si>
+    <t>FXI</t>
+  </si>
+  <si>
     <t>EWN</t>
   </si>
   <si>
+    <t>iShares MSCI Neth</t>
+  </si>
+  <si>
     <t>EWY</t>
   </si>
   <si>
-    <t>EWL</t>
+    <t>iShares MSCI Sout</t>
+  </si>
+  <si>
+    <t>ESR</t>
+  </si>
+  <si>
+    <t>iShares MSCI Emer</t>
+  </si>
+  <si>
+    <t>EEM</t>
   </si>
   <si>
     <t>EZA</t>
   </si>
   <si>
-    <t>ESR</t>
-  </si>
-  <si>
-    <t>FXI</t>
-  </si>
-  <si>
-    <t>EEM</t>
-  </si>
-  <si>
     <t>EFA</t>
   </si>
   <si>
+    <t>iShares MSCI EAFE</t>
+  </si>
+  <si>
+    <t>LATM</t>
+  </si>
+  <si>
+    <t>Market Vectors La</t>
+  </si>
+  <si>
     <t>BRF</t>
   </si>
   <si>
     <t>Market Vectors Br</t>
   </si>
   <si>
+    <t>ENOR</t>
+  </si>
+  <si>
+    <t>SPY</t>
+  </si>
+  <si>
+    <t>SPDR S&amp;P 500</t>
+  </si>
+  <si>
+    <t>ACWI</t>
+  </si>
+  <si>
+    <t>iShares MSCI ACWI</t>
+  </si>
+  <si>
+    <t>ERUS</t>
+  </si>
+  <si>
+    <t>iShares MSCI Russ</t>
+  </si>
+  <si>
     <t>EWT</t>
   </si>
   <si>
-    <t>ACWI</t>
-  </si>
-  <si>
-    <t>iShares MSCI ACWI</t>
-  </si>
-  <si>
-    <t>ENOR</t>
-  </si>
-  <si>
-    <t>LATM</t>
-  </si>
-  <si>
-    <t>ERUS</t>
-  </si>
-  <si>
-    <t>SPY</t>
+    <t>iShares MSCI Taiw</t>
+  </si>
+  <si>
+    <t>RSX</t>
+  </si>
+  <si>
+    <t>Market Vectors TR</t>
+  </si>
+  <si>
+    <t>EWI</t>
+  </si>
+  <si>
+    <t>iShares MSCI Ital</t>
+  </si>
+  <si>
+    <t>EWU</t>
+  </si>
+  <si>
+    <t>iShares MSCI Unit</t>
   </si>
   <si>
     <t>PEK</t>
   </si>
   <si>
-    <t>EWI</t>
-  </si>
-  <si>
-    <t>EWU</t>
-  </si>
-  <si>
-    <t>RSX</t>
+    <t>Market Vectors Ch</t>
   </si>
   <si>
     <t>EWM</t>
   </si>
   <si>
+    <t>iShares MSCI Mala</t>
+  </si>
+  <si>
     <t>ITF</t>
   </si>
   <si>
+    <t>iShares S&amp;P/TOPIX</t>
+  </si>
+  <si>
     <t>ECH</t>
   </si>
   <si>
+    <t>iShares MSCI Chil</t>
+  </si>
+  <si>
+    <t>EWC</t>
+  </si>
+  <si>
+    <t>iShares MSCI Cana</t>
+  </si>
+  <si>
     <t>EWJ</t>
   </si>
   <si>
-    <t>EWC</t>
+    <t>iShares MSCI Japa</t>
   </si>
   <si>
     <t>EIS</t>
   </si>
   <si>
+    <t>iShares MSCI Isra</t>
+  </si>
+  <si>
+    <t>ILF</t>
+  </si>
+  <si>
+    <t>iShares Latin Ame</t>
+  </si>
+  <si>
     <t>MES</t>
   </si>
   <si>
-    <t>ILF</t>
+    <t>Market Vectors Gu</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>iShares MSCI Fron</t>
+  </si>
+  <si>
+    <t>EFNL</t>
   </si>
   <si>
     <t>EWP</t>
   </si>
   <si>
-    <t>FM</t>
+    <t>iShares MSCI Spai</t>
   </si>
   <si>
     <t>EIDO</t>
   </si>
   <si>
-    <t>EFNL</t>
+    <t>MSCI Indonesia In</t>
   </si>
   <si>
     <t>IDX</t>
   </si>
   <si>
+    <t>Market Vectors In</t>
+  </si>
+  <si>
     <t>EWZ</t>
   </si>
   <si>
+    <t>iShares MSCI Braz</t>
+  </si>
+  <si>
     <t>EEML</t>
   </si>
   <si>
@@ -237,6 +378,9 @@
   </si>
   <si>
     <t>RSXJ</t>
+  </si>
+  <si>
+    <t>Market Vectors Ru</t>
   </si>
   <si>
     <t>IDXJ</t>
@@ -608,10 +752,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>0.655839325564</v>
+        <v>0.677659310687</v>
       </c>
       <c r="D2" t="n">
-        <v>3.28709068334</v>
+        <v>3.25878833559</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -619,895 +763,895 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>0.479023972603</v>
+        <v>0.52397260274</v>
       </c>
       <c r="D3" t="n">
-        <v>2.01595654394</v>
+        <v>2.16803723342</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>0.445578231293</v>
+        <v>0.507936507937</v>
       </c>
       <c r="D4" t="n">
-        <v>1.77551348916</v>
+        <v>2.05422525635</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>0.41586998088</v>
+        <v>0.4335499114</v>
       </c>
       <c r="D5" t="n">
-        <v>1.56193943754</v>
+        <v>1.52628589684</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>0.401461094122</v>
+        <v>0.414373088685</v>
       </c>
       <c r="D6" t="n">
-        <v>1.4583532525</v>
+        <v>1.39018342713</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>0.356065178033</v>
+        <v>0.386711281071</v>
       </c>
       <c r="D7" t="n">
-        <v>1.13199981224</v>
+        <v>1.19386100247</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C8" t="n">
-        <v>0.353219137626</v>
+        <v>0.360384108454</v>
       </c>
       <c r="D8" t="n">
-        <v>1.11153948986</v>
+        <v>1.00701079966</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C9" t="n">
-        <v>0.342429106474</v>
+        <v>0.345639379347</v>
       </c>
       <c r="D9" t="n">
-        <v>1.03396943312</v>
+        <v>0.90236395193</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C10" t="n">
-        <v>0.327998493692</v>
+        <v>0.345505617978</v>
       </c>
       <c r="D10" t="n">
-        <v>0.930227058644</v>
+        <v>0.90141461569</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C11" t="n">
-        <v>0.322978039636</v>
+        <v>0.342788171394</v>
       </c>
       <c r="D11" t="n">
-        <v>0.894134771183</v>
+        <v>0.88212825127</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C12" t="n">
-        <v>0.317613089509</v>
+        <v>0.332568807339</v>
       </c>
       <c r="D12" t="n">
-        <v>0.855565884783</v>
+        <v>0.809598995129</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C13" t="n">
-        <v>0.317333333333</v>
+        <v>0.325120514194</v>
       </c>
       <c r="D13" t="n">
-        <v>0.85355470408</v>
+        <v>0.756736687996</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C14" t="n">
-        <v>0.309575233981</v>
+        <v>0.324350336862</v>
       </c>
       <c r="D14" t="n">
-        <v>0.797781351947</v>
+        <v>0.75127055638</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C15" t="n">
-        <v>0.292942743009</v>
+        <v>0.321523809524</v>
       </c>
       <c r="D15" t="n">
-        <v>0.678209568481</v>
+        <v>0.731210019909</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C16" t="n">
-        <v>0.275229357798</v>
+        <v>0.316774658027</v>
       </c>
       <c r="D16" t="n">
-        <v>0.550867183958</v>
+        <v>0.697504162725</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C17" t="n">
-        <v>0.267039674466</v>
+        <v>0.312916111851</v>
       </c>
       <c r="D17" t="n">
-        <v>0.49199115368</v>
+        <v>0.670119143221</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C18" t="n">
-        <v>0.26652337453</v>
+        <v>0.28992878942</v>
       </c>
       <c r="D18" t="n">
-        <v>0.488279448424</v>
+        <v>0.506972651164</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C19" t="n">
-        <v>0.26404494382</v>
+        <v>0.283181085438</v>
       </c>
       <c r="D19" t="n">
-        <v>0.470461889969</v>
+        <v>0.459082591874</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C20" t="n">
-        <v>0.259541984733</v>
+        <v>0.271996785858</v>
       </c>
       <c r="D20" t="n">
-        <v>0.438089898915</v>
+        <v>0.379704958915</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C21" t="n">
-        <v>0.244334569427</v>
+        <v>0.267640505076</v>
       </c>
       <c r="D21" t="n">
-        <v>0.328763053461</v>
+        <v>0.348787398587</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C22" t="n">
-        <v>0.242887249737</v>
+        <v>0.263973577236</v>
       </c>
       <c r="D22" t="n">
-        <v>0.31835820208</v>
+        <v>0.322762339971</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C23" t="n">
-        <v>0.240256536754</v>
+        <v>0.261911170929</v>
       </c>
       <c r="D23" t="n">
-        <v>0.299445878985</v>
+        <v>0.308124952115</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C24" t="n">
-        <v>0.235606369947</v>
+        <v>0.261356565028</v>
       </c>
       <c r="D24" t="n">
-        <v>0.266015604503</v>
+        <v>0.304188782192</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C25" t="n">
-        <v>0.234993270525</v>
+        <v>0.259579728059</v>
       </c>
       <c r="D25" t="n">
-        <v>0.261608003052</v>
+        <v>0.291578147818</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C26" t="n">
-        <v>0.232731798382</v>
+        <v>0.257030093735</v>
       </c>
       <c r="D26" t="n">
-        <v>0.245350170246</v>
+        <v>0.273482786892</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C27" t="n">
-        <v>0.232215447154</v>
+        <v>0.251327072274</v>
       </c>
       <c r="D27" t="n">
-        <v>0.241638096252</v>
+        <v>0.233007087813</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C28" t="n">
-        <v>0.229264669473</v>
+        <v>0.238672286617</v>
       </c>
       <c r="D28" t="n">
-        <v>0.220424812528</v>
+        <v>0.143193065589</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C29" t="n">
-        <v>0.22763915547</v>
+        <v>0.236710586097</v>
       </c>
       <c r="D29" t="n">
-        <v>0.208738913607</v>
+        <v>0.129270410643</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>0.220833333333</v>
+        <v>0.235700575816</v>
       </c>
       <c r="D30" t="n">
-        <v>0.159811528512</v>
+        <v>0.122102127566</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C31" t="n">
-        <v>0.219441770934</v>
+        <v>0.225920471281</v>
       </c>
       <c r="D31" t="n">
-        <v>0.149807518997</v>
+        <v>0.052690400665</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C32" t="n">
-        <v>0.21762835075</v>
+        <v>0.225595238095</v>
       </c>
       <c r="D32" t="n">
-        <v>0.136770753432</v>
+        <v>0.050382143426</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="C33" t="n">
-        <v>0.210143702451</v>
+        <v>0.224254090472</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0829632541733</v>
+        <v>0.0408636999107</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C34" t="n">
-        <v>0.193121693122</v>
+        <v>0.208553791887</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.0394087956395</v>
+        <v>-0.0705650515681</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C35" t="n">
-        <v>0.19145802651</v>
+        <v>0.207785234899</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.0513689755212</v>
+        <v>-0.0760196832191</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="C36" t="n">
-        <v>0.190604026846</v>
+        <v>0.20338123415</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.0575084204827</v>
+        <v>-0.107275923495</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="C37" t="n">
-        <v>0.187552213868</v>
+        <v>0.200292397661</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.0794480518438</v>
+        <v>-0.12919813037</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C38" t="n">
-        <v>0.187186629526</v>
+        <v>0.197236779419</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.0820762553883</v>
+        <v>-0.150884579444</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="C39" t="n">
-        <v>0.186411149826</v>
+        <v>0.193871866295</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.0876512165296</v>
+        <v>-0.174766167821</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>0.167557066537</v>
+        <v>0.193664795509</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.2231941348</v>
+        <v>-0.176235798416</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="C41" t="n">
-        <v>0.16680032077</v>
+        <v>0.192132269099</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.228634416786</v>
+        <v>-0.187112502675</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="C42" t="n">
-        <v>0.162934730824</v>
+        <v>0.190869354055</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.256424330199</v>
+        <v>-0.196075710973</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="C43" t="n">
-        <v>0.160451422964</v>
+        <v>0.189401373896</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.274276950728</v>
+        <v>-0.206494315147</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="C44" t="n">
-        <v>0.159879459195</v>
+        <v>0.187282229965</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.278388825972</v>
+        <v>-0.221534383407</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="C45" t="n">
-        <v>0.153603034134</v>
+        <v>0.176221623701</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.32351034984</v>
+        <v>-0.300034135493</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="C46" t="n">
-        <v>0.153516295026</v>
+        <v>0.172384219554</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.324133921492</v>
+        <v>-0.327269104992</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="C47" t="n">
-        <v>0.152956298201</v>
+        <v>0.168380462725</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.328159765801</v>
+        <v>-0.355684719019</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="C48" t="n">
-        <v>0.150442477876</v>
+        <v>0.166561314791</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.346231741911</v>
+        <v>-0.368595644369</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="C49" t="n">
-        <v>0.147951441578</v>
+        <v>0.157056145675</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.364139922552</v>
+        <v>-0.436056089245</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="C50" t="n">
-        <v>0.121532364597</v>
+        <v>0.145838837517</v>
       </c>
       <c r="D50" t="n">
-        <v>-0.554067947012</v>
+        <v>-0.515667991933</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="C51" t="n">
-        <v>0.112988384372</v>
+        <v>0.138859556494</v>
       </c>
       <c r="D51" t="n">
-        <v>-0.615491034821</v>
+        <v>-0.56520160853</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0918253079507</v>
+        <v>0.105647330004</v>
       </c>
       <c r="D52" t="n">
-        <v>-0.767633416594</v>
+        <v>-0.800916675459</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="C53" t="n">
-        <v>0.0910487898579</v>
+        <v>0.104143337066</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.773215842787</v>
+        <v>-0.811590870882</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="C54" t="n">
-        <v>0.0871821484172</v>
+        <v>0.101712506487</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.801013315448</v>
+        <v>-0.828843053384</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="C55" t="n">
-        <v>0.0663507109005</v>
+        <v>0.0916767189385</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.95077152907</v>
+        <v>-0.900069423417</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="C56" t="n">
-        <v>0.0576598311218</v>
+        <v>0.0837282780411</v>
       </c>
       <c r="D56" t="n">
-        <v>-1.01325068488</v>
+        <v>-0.956481398045</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>108</v>
       </c>
       <c r="C57" t="n">
-        <v>0.0539881574364</v>
+        <v>0.072872949256</v>
       </c>
       <c r="D57" t="n">
-        <v>-1.03964652491</v>
+        <v>-1.03352424706</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.0537962609691</v>
+        <v>0.0704113924051</v>
       </c>
       <c r="D58" t="n">
-        <v>-1.04102607791</v>
+        <v>-1.05099450122</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="C59" t="n">
-        <v>0.0452504317789</v>
+        <v>0.0651340996169</v>
       </c>
       <c r="D59" t="n">
-        <v>-1.10246245801</v>
+        <v>-1.08844870271</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="C60" t="n">
-        <v>0.0356012658228</v>
+        <v>0.0632124352332</v>
       </c>
       <c r="D60" t="n">
-        <v>-1.17183077959</v>
+        <v>-1.10208721167</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>115</v>
       </c>
       <c r="C61" t="n">
-        <v>0.0239542366822</v>
+        <v>0.0375402216661</v>
       </c>
       <c r="D61" t="n">
-        <v>-1.2555618364</v>
+        <v>-1.2842890144</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>117</v>
       </c>
       <c r="C62" t="n">
-        <v>0.00358808754934</v>
+        <v>0.0258342303552</v>
       </c>
       <c r="D62" t="n">
-        <v>-1.40197506928</v>
+        <v>-1.3673692176</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.00493545937737</v>
+        <v>0.0159453302961</v>
       </c>
       <c r="D63" t="n">
-        <v>-1.46325126112</v>
+        <v>-1.4375530922</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.0146506386176</v>
+        <v>-0.00525920360631</v>
       </c>
       <c r="D64" t="n">
-        <v>-1.53309415539</v>
+        <v>-1.58804671025</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="C65" t="n">
-        <v>-0.0249520153551</v>
+        <v>-0.0185540626999</v>
       </c>
       <c r="D65" t="n">
-        <v>-1.60715125187</v>
+        <v>-1.68240348582</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>115</v>
       </c>
       <c r="C66" t="n">
-        <v>-0.261710794297</v>
+        <v>-0.228105906314</v>
       </c>
       <c r="D66" t="n">
-        <v>-3.309221585</v>
+        <v>-3.16964273661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>